<commit_message>
Writeup updates - compare with EKF - comapre with Radar/Lidar only data -
</commit_message>
<xml_diff>
--- a/laser_nis_data.xlsx
+++ b/laser_nis_data.xlsx
@@ -19,16 +19,28 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t xml:space="preserve">stdev</t>
+  </si>
+  <si>
+    <t xml:space="preserve">95 percentile</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -44,6 +56,29 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="13"/>
@@ -159,7 +194,7 @@
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FFFF420E"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF004586"/>
@@ -175,7 +210,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -237,6 +272,7 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1003,11 +1039,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="13551387"/>
-        <c:axId val="79979813"/>
+        <c:axId val="49577739"/>
+        <c:axId val="91203765"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="13551387"/>
+        <c:axId val="49577739"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1080,14 +1116,1844 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="79979813"/>
+        <c:crossAx val="91203765"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="79979813"/>
+        <c:axId val="91203765"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>NIS</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="49577739"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="0" sz="1300" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:rPr>
+              <a:t>Lidar NIS values</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>nis</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>nis</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>laser_nis!$A$1:$A$249</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="249"/>
+                <c:pt idx="0">
+                  <c:v>0.00837758</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.415162</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.528248</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.123013</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.665194</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.42109</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.103737</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10.2238</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.10726</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.87339</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.13795</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.204041</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.00856</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.468915</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.404656</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.872109</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.668533</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.42686</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.2584</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.20197</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.92123</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.351812</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.69419</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.29493</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.55288</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.867146</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.654461</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2.2135</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.18436</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.7126</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.209416</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.422191</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.490249</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.645257</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.214676</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1.75289</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.714453</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.596026</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2.08158</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>4.00421</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1.20966</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1.41029</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>3.90963</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>4.15601</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2.97678</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.736758</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.916788</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2.01223</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.000309057</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>4.66485</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1.1558</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1.78612</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1.04822</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1.28241</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.351753</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1.26163</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>2.1179</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>3.54326</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.0116242</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.69474</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.141024</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1.84964</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>3.86914</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.905477</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1.08907</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.492611</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.322419</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>2.68624</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.869985</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.776416</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>1.36381</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>1.87823</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.644589</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.715594</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>1.71545</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.167072</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>1.94251</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.138228</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>1.93104</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.700856</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.611702</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>3.36837</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>1.67462</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>1.00685</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>2.29372</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>2.79693</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.135288</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>3.51768</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.704121</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.346182</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>0.822497</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>1.39966</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>1.94925</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>0.715812</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>1.12465</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>2.00093</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>2.6369</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>1.19003</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>6.1597</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>0.0628434</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>0.514661</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>2.24448</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>1.81333</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>0.811353</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>2.44433</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>0.444718</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>0.890024</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>3.73869</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>1.36683</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>3.46589</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>0.34436</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>0.531461</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>4.33939</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>2.51847</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>0.970702</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>2.03431</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>0.807896</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>4.02519</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>0.172224</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>0.747674</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>0.767243</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>0.381913</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>2.44715</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>0.303965</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>1.69711</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>0.630232</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>2.22888</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>2.65413</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>0.652555</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>0.0042087</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>1.24876</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>0.649357</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>1.53766</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>4.82971</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>3.84188</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>1.47421</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>1.56538</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>2.81553</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>1.35565</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>1.16782</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>0.407032</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>0.58575</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>2.25151</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>1.35515</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>4.92458</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>0.543325</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>1.2757</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>0.242473</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>1.83726</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>0.122655</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>4.71235</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>0.509753</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>0.718638</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>3.75629</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>3.70803</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>3.01559</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>3.01542</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>0.751285</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>1.83372</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>4.30254</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>1.95784</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>0.849211</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>0.607689</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>2.1244</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>5.22671</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>2.06732</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>0.55331</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>1.43116</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>0.441346</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>0.220825</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>2.33451</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>0.21951</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>3.21874</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>1.50512</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>14.3183</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>0.841376</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>1.45422</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>1.78028</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>0.178722</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>1.02898</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>6.06534</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>2.015</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>0.85051</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>2.02126</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>3.68669</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>5.83214</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>2.28219</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>0.265347</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>0.510386</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>0.572659</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>0.644562</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>2.25174</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>5.21646</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>1.96039</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>5.09883</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>0.948436</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>1.56238</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>0.0941179</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>0.343458</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>3.0628</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>1.49659</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>2.48274</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>0.186712</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>0.355532</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>0.771331</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>0.128766</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>1.57171</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>0.314361</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>3.32487</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>2.45089</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>0.269065</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>1.1687</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>1.64306</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>0.14033</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>0.0684354</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>4.64674</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>1.26798</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>0.165898</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>1.70706</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>0.0457417</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>4.86962</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>2.77525</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>1.54374</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>0.466843</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>0.679849</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>6.39539</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>0.883085</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>3.55732</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>1.26129</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>1.39788</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>1.15208</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>0.703652</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>1.78839</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>0.183213</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>2.34616</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>7.66068</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>0.596106</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>3.8435</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>1.95406</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>1.99505</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>0.771081</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>2.92469</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>0.911379</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>1.95902</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>0.650528</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>0.979535</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>5.34798</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>5.26709</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>0.60308</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>95_prec</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>95_prec</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>laser_nis!$B$1:$B$249</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="249"/>
+                <c:pt idx="0">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>3.53</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="100"/>
+        <c:overlap val="0"/>
+        <c:axId val="15383103"/>
+        <c:axId val="68247729"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="15383103"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:uFill>
+                      <a:solidFill>
+                        <a:srgbClr val="ffffff"/>
+                      </a:solidFill>
+                    </a:uFill>
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Time steps</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:uFill>
+                  <a:solidFill>
+                    <a:srgbClr val="ffffff"/>
+                  </a:solidFill>
+                </a:uFill>
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="68247729"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="68247729"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1169,7 +3035,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="13551387"/>
+        <c:crossAx val="15383103"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1210,16 +3076,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>35640</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>38160</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>421200</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>143640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>209520</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>95760</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>594360</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>38160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1227,12 +3093,42 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="871920" y="38160"/>
-        <a:ext cx="12365640" cy="3633840"/>
+        <a:off x="2040120" y="306000"/>
+        <a:ext cx="12174840" cy="3633480"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>306720</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>124560</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>20160</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>114840</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="1" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="5926320" y="4350960"/>
+        <a:ext cx="10114560" cy="3241440"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1246,1261 +3142,2270 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A249"/>
+  <dimension ref="A1:F249"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N29" activeCellId="0" sqref="N29"/>
+      <selection pane="topLeft" activeCell="D35" activeCellId="0" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.8520408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="n">
         <v>0.00837758</v>
       </c>
+      <c r="B1" s="0" t="n">
+        <v>3.53</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
         <v>0.415162</v>
       </c>
+      <c r="B2" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>0.528248</v>
       </c>
+      <c r="B3" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>0.123013</v>
       </c>
+      <c r="B4" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>0.665194</v>
       </c>
+      <c r="B5" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>5.42109</v>
       </c>
+      <c r="B6" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>0.103737</v>
       </c>
+      <c r="B7" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>10.2238</v>
       </c>
+      <c r="B8" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>3.10726</v>
       </c>
+      <c r="B9" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>1.87339</v>
       </c>
+      <c r="B10" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>3.13795</v>
       </c>
+      <c r="B11" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>0.204041</v>
       </c>
+      <c r="B12" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>3.00856</v>
       </c>
+      <c r="B13" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <v>0.468915</v>
       </c>
+      <c r="B14" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <v>0.404656</v>
       </c>
+      <c r="B15" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <v>0.872109</v>
       </c>
+      <c r="B16" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
         <v>0.668533</v>
       </c>
+      <c r="B17" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
         <v>3.42686</v>
       </c>
+      <c r="B18" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
         <v>1.2584</v>
       </c>
+      <c r="B19" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
         <v>1.20197</v>
       </c>
+      <c r="B20" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
         <v>1.92123</v>
       </c>
+      <c r="B21" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
         <v>0.351812</v>
       </c>
+      <c r="B22" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
         <v>0.69419</v>
       </c>
+      <c r="B23" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="n">
         <v>3.29493</v>
       </c>
+      <c r="B24" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
         <v>2.55288</v>
       </c>
+      <c r="B25" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
         <v>0.867146</v>
       </c>
+      <c r="B26" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
         <v>0.654461</v>
       </c>
+      <c r="B27" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
         <v>2.2135</v>
       </c>
+      <c r="B28" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="n">
         <v>1.18436</v>
       </c>
+      <c r="B29" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
+      <c r="E29" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="F29" s="0" t="n">
+        <f aca="false">STDEV(A1:A249)</f>
+        <v>1.76227415052563</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
         <v>0.7126</v>
       </c>
+      <c r="B30" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
+      <c r="E30" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="F30" s="0" t="n">
+        <f aca="false">2*F29</f>
+        <v>3.52454830105126</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
         <v>0.209416</v>
       </c>
+      <c r="B31" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
         <v>0.422191</v>
       </c>
+      <c r="B32" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
         <v>0.490249</v>
       </c>
+      <c r="B33" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
         <v>0.645257</v>
       </c>
+      <c r="B34" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
         <v>0.214676</v>
       </c>
+      <c r="B35" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
         <v>1.75289</v>
       </c>
+      <c r="B36" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
         <v>0.714453</v>
       </c>
+      <c r="B37" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
         <v>0.596026</v>
       </c>
+      <c r="B38" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
         <v>2.08158</v>
       </c>
+      <c r="B39" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="n">
         <v>4.00421</v>
       </c>
+      <c r="B40" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="n">
         <v>1.20966</v>
       </c>
+      <c r="B41" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="n">
         <v>1.41029</v>
       </c>
+      <c r="B42" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="n">
         <v>3.90963</v>
       </c>
+      <c r="B43" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="n">
         <v>4.15601</v>
       </c>
+      <c r="B44" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="n">
         <v>2.97678</v>
       </c>
+      <c r="B45" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="n">
         <v>0.736758</v>
       </c>
+      <c r="B46" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="n">
         <v>0.916788</v>
       </c>
+      <c r="B47" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="n">
         <v>2.01223</v>
       </c>
+      <c r="B48" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="n">
         <v>0.000309057</v>
       </c>
+      <c r="B49" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="n">
         <v>4.66485</v>
       </c>
+      <c r="B50" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="n">
         <v>1.1558</v>
       </c>
+      <c r="B51" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="n">
         <v>1.78612</v>
       </c>
+      <c r="B52" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="n">
         <v>1.04822</v>
       </c>
+      <c r="B53" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="n">
         <v>1.28241</v>
       </c>
+      <c r="B54" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="n">
         <v>0.351753</v>
       </c>
+      <c r="B55" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="n">
         <v>1.26163</v>
       </c>
+      <c r="B56" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="n">
         <v>2.1179</v>
       </c>
+      <c r="B57" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="n">
         <v>3.54326</v>
       </c>
+      <c r="B58" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="n">
         <v>0.0116242</v>
       </c>
+      <c r="B59" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="n">
         <v>0.69474</v>
       </c>
+      <c r="B60" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="n">
         <v>0.141024</v>
       </c>
+      <c r="B61" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="n">
         <v>1.84964</v>
       </c>
+      <c r="B62" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="n">
         <v>3.86914</v>
       </c>
+      <c r="B63" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="n">
         <v>0.905477</v>
       </c>
+      <c r="B64" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="n">
         <v>1.08907</v>
       </c>
+      <c r="B65" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="n">
         <v>0.492611</v>
       </c>
+      <c r="B66" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="n">
         <v>0.322419</v>
       </c>
+      <c r="B67" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="n">
         <v>2.68624</v>
       </c>
+      <c r="B68" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="n">
         <v>0.869985</v>
       </c>
+      <c r="B69" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="n">
         <v>0.776416</v>
       </c>
+      <c r="B70" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="n">
         <v>1.36381</v>
       </c>
+      <c r="B71" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="0" t="n">
         <v>1.87823</v>
       </c>
+      <c r="B72" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="0" t="n">
         <v>0.644589</v>
       </c>
+      <c r="B73" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="0" t="n">
         <v>0.715594</v>
       </c>
+      <c r="B74" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="0" t="n">
         <v>1.71545</v>
       </c>
+      <c r="B75" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="0" t="n">
         <v>0.167072</v>
       </c>
+      <c r="B76" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="n">
         <v>1.94251</v>
       </c>
+      <c r="B77" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="0" t="n">
         <v>0.138228</v>
       </c>
+      <c r="B78" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="0" t="n">
         <v>1.93104</v>
       </c>
+      <c r="B79" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="0" t="n">
         <v>0.700856</v>
       </c>
+      <c r="B80" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="0" t="n">
         <v>0.611702</v>
       </c>
+      <c r="B81" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="0" t="n">
         <v>3.36837</v>
       </c>
+      <c r="B82" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="n">
         <v>1.67462</v>
       </c>
+      <c r="B83" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="n">
         <v>1.00685</v>
       </c>
+      <c r="B84" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="0" t="n">
         <v>2.29372</v>
       </c>
+      <c r="B85" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="0" t="n">
         <v>2.79693</v>
       </c>
+      <c r="B86" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="0" t="n">
         <v>0.135288</v>
       </c>
+      <c r="B87" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="n">
         <v>3.51768</v>
       </c>
+      <c r="B88" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="0" t="n">
         <v>0.704121</v>
       </c>
+      <c r="B89" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="0" t="n">
         <v>0.346182</v>
       </c>
+      <c r="B90" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="0" t="n">
         <v>0.822497</v>
       </c>
+      <c r="B91" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="0" t="n">
         <v>1.39966</v>
       </c>
+      <c r="B92" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="n">
         <v>1.94925</v>
       </c>
+      <c r="B93" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="0" t="n">
         <v>0.715812</v>
       </c>
+      <c r="B94" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="n">
         <v>1.12465</v>
       </c>
+      <c r="B95" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="n">
         <v>2.00093</v>
       </c>
+      <c r="B96" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="0" t="n">
         <v>2.6369</v>
       </c>
+      <c r="B97" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="0" t="n">
         <v>1.19003</v>
       </c>
+      <c r="B98" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="n">
         <v>6.1597</v>
       </c>
+      <c r="B99" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="n">
         <v>0.0628434</v>
       </c>
+      <c r="B100" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="0" t="n">
         <v>0.514661</v>
       </c>
+      <c r="B101" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="n">
         <v>2.24448</v>
       </c>
+      <c r="B102" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="0" t="n">
         <v>1.81333</v>
       </c>
+      <c r="B103" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="0" t="n">
         <v>0.811353</v>
       </c>
+      <c r="B104" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="0" t="n">
         <v>2.44433</v>
       </c>
+      <c r="B105" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="0" t="n">
         <v>0.444718</v>
       </c>
+      <c r="B106" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="n">
         <v>0.890024</v>
       </c>
+      <c r="B107" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="0" t="n">
         <v>3.73869</v>
       </c>
+      <c r="B108" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="n">
         <v>1.36683</v>
       </c>
+      <c r="B109" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="n">
         <v>3.46589</v>
       </c>
+      <c r="B110" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="0" t="n">
         <v>0.34436</v>
       </c>
+      <c r="B111" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="n">
         <v>0.531461</v>
       </c>
+      <c r="B112" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="n">
         <v>4.33939</v>
       </c>
+      <c r="B113" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="n">
         <v>2.51847</v>
       </c>
+      <c r="B114" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="n">
         <v>0.970702</v>
       </c>
+      <c r="B115" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="0" t="n">
         <v>2.03431</v>
       </c>
+      <c r="B116" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="n">
         <v>0.807896</v>
       </c>
+      <c r="B117" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="0" t="n">
         <v>4.02519</v>
       </c>
+      <c r="B118" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="n">
         <v>0.172224</v>
       </c>
+      <c r="B119" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="n">
         <v>0.747674</v>
       </c>
+      <c r="B120" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="0" t="n">
         <v>0.767243</v>
       </c>
+      <c r="B121" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="n">
         <v>0.381913</v>
       </c>
+      <c r="B122" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="n">
         <v>2.44715</v>
       </c>
+      <c r="B123" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="n">
         <v>0.303965</v>
       </c>
+      <c r="B124" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="n">
         <v>1.69711</v>
       </c>
+      <c r="B125" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="0" t="n">
         <v>0.630232</v>
       </c>
+      <c r="B126" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="0" t="n">
         <v>2.22888</v>
       </c>
+      <c r="B127" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="0" t="n">
         <v>2.65413</v>
       </c>
+      <c r="B128" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="n">
         <v>0.652555</v>
       </c>
+      <c r="B129" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="0" t="n">
         <v>0.0042087</v>
       </c>
+      <c r="B130" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="n">
         <v>1.24876</v>
       </c>
+      <c r="B131" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="n">
         <v>0.649357</v>
       </c>
+      <c r="B132" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="0" t="n">
         <v>1.53766</v>
       </c>
+      <c r="B133" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="0" t="n">
         <v>4.82971</v>
       </c>
+      <c r="B134" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="n">
         <v>3.84188</v>
       </c>
+      <c r="B135" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="0" t="n">
         <v>1.47421</v>
       </c>
+      <c r="B136" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="0" t="n">
         <v>1.56538</v>
       </c>
+      <c r="B137" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="0" t="n">
         <v>2.81553</v>
       </c>
+      <c r="B138" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="0" t="n">
         <v>1.35565</v>
       </c>
+      <c r="B139" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="n">
         <v>1.16782</v>
       </c>
+      <c r="B140" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="n">
         <v>0.407032</v>
       </c>
+      <c r="B141" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="n">
         <v>0.58575</v>
       </c>
+      <c r="B142" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="n">
         <v>2.25151</v>
       </c>
+      <c r="B143" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="n">
         <v>1.35515</v>
       </c>
+      <c r="B144" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="0" t="n">
         <v>4.92458</v>
       </c>
+      <c r="B145" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="n">
         <v>0.543325</v>
       </c>
+      <c r="B146" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="n">
         <v>1.2757</v>
       </c>
+      <c r="B147" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="n">
         <v>0.242473</v>
       </c>
+      <c r="B148" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="n">
         <v>1.83726</v>
       </c>
+      <c r="B149" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="n">
         <v>0.122655</v>
       </c>
+      <c r="B150" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="0" t="n">
         <v>4.71235</v>
       </c>
+      <c r="B151" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="0" t="n">
         <v>0.509753</v>
       </c>
+      <c r="B152" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="0" t="n">
         <v>0.718638</v>
       </c>
+      <c r="B153" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="0" t="n">
         <v>3.75629</v>
       </c>
+      <c r="B154" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="0" t="n">
         <v>3.70803</v>
       </c>
+      <c r="B155" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="0" t="n">
         <v>3.01559</v>
       </c>
+      <c r="B156" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="0" t="n">
         <v>3.01542</v>
       </c>
+      <c r="B157" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="0" t="n">
         <v>0.751285</v>
       </c>
+      <c r="B158" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="0" t="n">
         <v>1.83372</v>
       </c>
+      <c r="B159" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="0" t="n">
         <v>4.30254</v>
       </c>
+      <c r="B160" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="0" t="n">
         <v>1.95784</v>
       </c>
+      <c r="B161" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="0" t="n">
         <v>0.849211</v>
       </c>
+      <c r="B162" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="0" t="n">
         <v>0.607689</v>
       </c>
+      <c r="B163" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="0" t="n">
         <v>2.1244</v>
       </c>
+      <c r="B164" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="0" t="n">
         <v>5.22671</v>
       </c>
+      <c r="B165" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="0" t="n">
         <v>2.06732</v>
       </c>
+      <c r="B166" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="0" t="n">
         <v>0.55331</v>
       </c>
+      <c r="B167" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="0" t="n">
         <v>1.43116</v>
       </c>
+      <c r="B168" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="0" t="n">
         <v>0.441346</v>
       </c>
+      <c r="B169" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="0" t="n">
         <v>0.220825</v>
       </c>
+      <c r="B170" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="0" t="n">
         <v>2.33451</v>
       </c>
+      <c r="B171" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="0" t="n">
         <v>0.21951</v>
       </c>
+      <c r="B172" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="0" t="n">
         <v>3.21874</v>
       </c>
+      <c r="B173" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="0" t="n">
         <v>1.50512</v>
       </c>
+      <c r="B174" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="0" t="n">
         <v>14.3183</v>
       </c>
+      <c r="B175" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="0" t="n">
         <v>0.841376</v>
       </c>
+      <c r="B176" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="0" t="n">
         <v>1.45422</v>
       </c>
+      <c r="B177" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="0" t="n">
         <v>1.78028</v>
       </c>
+      <c r="B178" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="0" t="n">
         <v>0.178722</v>
       </c>
+      <c r="B179" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="0" t="n">
         <v>1.02898</v>
       </c>
+      <c r="B180" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="0" t="n">
         <v>6.06534</v>
       </c>
+      <c r="B181" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="0" t="n">
         <v>2.015</v>
       </c>
+      <c r="B182" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="0" t="n">
         <v>0.85051</v>
       </c>
+      <c r="B183" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="0" t="n">
         <v>2.02126</v>
       </c>
+      <c r="B184" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="0" t="n">
         <v>3.68669</v>
       </c>
+      <c r="B185" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="0" t="n">
         <v>5.83214</v>
       </c>
+      <c r="B186" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="0" t="n">
         <v>2.28219</v>
       </c>
+      <c r="B187" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="0" t="n">
         <v>0.265347</v>
       </c>
+      <c r="B188" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="0" t="n">
         <v>0.510386</v>
       </c>
+      <c r="B189" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="0" t="n">
         <v>0.572659</v>
       </c>
+      <c r="B190" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="0" t="n">
         <v>0.644562</v>
       </c>
+      <c r="B191" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="0" t="n">
         <v>2.25174</v>
       </c>
+      <c r="B192" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="0" t="n">
         <v>5.21646</v>
       </c>
+      <c r="B193" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="0" t="n">
         <v>1.96039</v>
       </c>
+      <c r="B194" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="0" t="n">
         <v>5.09883</v>
       </c>
+      <c r="B195" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="0" t="n">
         <v>0.948436</v>
       </c>
+      <c r="B196" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="0" t="n">
         <v>1.56238</v>
       </c>
+      <c r="B197" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="0" t="n">
         <v>0.0941179</v>
       </c>
+      <c r="B198" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="0" t="n">
         <v>0.343458</v>
       </c>
+      <c r="B199" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="0" t="n">
         <v>3.0628</v>
       </c>
+      <c r="B200" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="0" t="n">
         <v>1.49659</v>
       </c>
+      <c r="B201" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="0" t="n">
         <v>2.48274</v>
       </c>
+      <c r="B202" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="0" t="n">
         <v>0.186712</v>
       </c>
+      <c r="B203" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="0" t="n">
         <v>0.355532</v>
       </c>
+      <c r="B204" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="0" t="n">
         <v>0.771331</v>
       </c>
+      <c r="B205" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A206" s="0" t="n">
         <v>0.128766</v>
       </c>
+      <c r="B206" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A207" s="0" t="n">
         <v>1.57171</v>
       </c>
+      <c r="B207" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A208" s="0" t="n">
         <v>0.314361</v>
       </c>
+      <c r="B208" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A209" s="0" t="n">
         <v>3.32487</v>
       </c>
+      <c r="B209" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A210" s="0" t="n">
         <v>2.45089</v>
       </c>
+      <c r="B210" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A211" s="0" t="n">
         <v>0.269065</v>
       </c>
+      <c r="B211" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A212" s="0" t="n">
         <v>1.1687</v>
       </c>
+      <c r="B212" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A213" s="0" t="n">
         <v>1.64306</v>
       </c>
+      <c r="B213" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A214" s="0" t="n">
         <v>0.14033</v>
       </c>
+      <c r="B214" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A215" s="0" t="n">
         <v>0.0684354</v>
       </c>
+      <c r="B215" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A216" s="0" t="n">
         <v>4.64674</v>
       </c>
+      <c r="B216" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A217" s="0" t="n">
         <v>1.26798</v>
       </c>
+      <c r="B217" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A218" s="0" t="n">
         <v>0.165898</v>
       </c>
+      <c r="B218" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A219" s="0" t="n">
         <v>1.70706</v>
       </c>
+      <c r="B219" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A220" s="0" t="n">
         <v>0.0457417</v>
       </c>
+      <c r="B220" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A221" s="0" t="n">
         <v>4.86962</v>
       </c>
+      <c r="B221" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A222" s="0" t="n">
         <v>2.77525</v>
       </c>
+      <c r="B222" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A223" s="0" t="n">
         <v>1.54374</v>
       </c>
+      <c r="B223" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A224" s="0" t="n">
         <v>0.466843</v>
       </c>
+      <c r="B224" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="0" t="n">
         <v>0.679849</v>
       </c>
+      <c r="B225" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A226" s="0" t="n">
         <v>6.39539</v>
       </c>
+      <c r="B226" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A227" s="0" t="n">
         <v>0.883085</v>
       </c>
+      <c r="B227" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="0" t="n">
         <v>3.55732</v>
       </c>
+      <c r="B228" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A229" s="0" t="n">
         <v>1.26129</v>
       </c>
+      <c r="B229" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A230" s="0" t="n">
         <v>1.39788</v>
       </c>
+      <c r="B230" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A231" s="0" t="n">
         <v>1.15208</v>
       </c>
+      <c r="B231" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A232" s="0" t="n">
         <v>0.703652</v>
       </c>
+      <c r="B232" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A233" s="0" t="n">
         <v>1.78839</v>
       </c>
+      <c r="B233" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A234" s="0" t="n">
         <v>0.183213</v>
       </c>
+      <c r="B234" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="0" t="n">
         <v>2.34616</v>
       </c>
+      <c r="B235" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A236" s="0" t="n">
         <v>7.66068</v>
       </c>
+      <c r="B236" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A237" s="0" t="n">
         <v>0.596106</v>
       </c>
+      <c r="B237" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="0" t="n">
         <v>3.8435</v>
       </c>
+      <c r="B238" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A239" s="0" t="n">
         <v>1.95406</v>
       </c>
+      <c r="B239" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A240" s="0" t="n">
         <v>1.99505</v>
       </c>
+      <c r="B240" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="0" t="n">
         <v>0.771081</v>
       </c>
+      <c r="B241" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A242" s="0" t="n">
         <v>2.92469</v>
       </c>
+      <c r="B242" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A243" s="0" t="n">
         <v>0.911379</v>
       </c>
+      <c r="B243" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="0" t="n">
         <v>1.95902</v>
       </c>
+      <c r="B244" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A245" s="0" t="n">
         <v>0.650528</v>
       </c>
+      <c r="B245" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A246" s="0" t="n">
         <v>0.979535</v>
       </c>
+      <c r="B246" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A247" s="0" t="n">
         <v>5.34798</v>
       </c>
+      <c r="B247" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A248" s="0" t="n">
         <v>5.26709</v>
       </c>
+      <c r="B248" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
+      </c>
     </row>
     <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A249" s="0" t="n">
         <v>0.60308</v>
+      </c>
+      <c r="B249" s="0" t="n">
+        <f aca="false">$B$1</f>
+        <v>3.53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>